<commit_message>
commit drivers and shifts initialise from excel
</commit_message>
<xml_diff>
--- a/Parser/daily_M.xlsx
+++ b/Parser/daily_M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jp/Library/Mobile Documents/com~apple~CloudDocs/testMVP/CDEV3300-Gate-Gourmet-Scheduling/Parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D675B8-2D16-3749-B496-2A0AB98F2F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DFF283-9800-7D4D-93DA-7D7FC7EF6531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{8740E76B-EDAF-2240-BEB8-3D4AC43AF0EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
   <si>
     <t>UA6 LD</t>
   </si>
@@ -685,6 +685,27 @@
   </si>
   <si>
     <t>TG PS;LD</t>
+  </si>
+  <si>
+    <t>Task Requirement</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>04:00-15:30</t>
+  </si>
+  <si>
+    <t>05:30-16:30</t>
+  </si>
+  <si>
+    <t>05:00-16:30</t>
+  </si>
+  <si>
+    <t>06:00-17:00</t>
+  </si>
+  <si>
+    <t>08:00-17:30</t>
   </si>
 </sst>
 </file>
@@ -3116,18 +3137,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407072A9-3406-3A4A-863F-47DC030259EB}">
-  <dimension ref="A1:CO86"/>
+  <dimension ref="A1:CP86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="CO14" sqref="CO14"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="CO2" sqref="CO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30"/>
   <cols>
-    <col min="93" max="93" width="44.83203125" style="274" customWidth="1"/>
+    <col min="93" max="94" width="44.83203125" style="274" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="1" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A1" s="244"/>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -3264,9 +3285,14 @@
       <c r="CL1" s="9"/>
       <c r="CM1" s="9"/>
       <c r="CN1" s="12"/>
-      <c r="CO1" s="265"/>
+      <c r="CO1" s="265" t="s">
+        <v>121</v>
+      </c>
+      <c r="CP1" s="265" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="2" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="2" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A2" s="245"/>
       <c r="B2" s="13">
         <v>3</v>
@@ -3278,14 +3304,14 @@
       <c r="E2" s="16"/>
       <c r="F2" s="17">
         <f>SUM(D3:E3)</f>
-        <v>12</v>
+        <v>-7</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="19">
         <f>E3</f>
-        <v>2.5</v>
+        <v>-7</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="21" t="s">
@@ -3386,20 +3412,23 @@
       <c r="CO2" s="266" t="s">
         <v>116</v>
       </c>
+      <c r="CP2" s="266" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="3" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="3" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A3" s="246"/>
       <c r="B3" s="42"/>
       <c r="C3" s="43">
         <v>1</v>
       </c>
       <c r="D3" s="44">
-        <f>SUM(I3:CN3)</f>
-        <v>9.5</v>
+        <f>SUM(I4:CN4)</f>
+        <v>0</v>
       </c>
       <c r="E3" s="15">
         <f>SUM(D3-7)</f>
-        <v>2.5</v>
+        <v>-7</v>
       </c>
       <c r="F3" s="45"/>
       <c r="G3" s="46"/>
@@ -3565,8 +3594,9 @@
       <c r="CM3" s="59"/>
       <c r="CN3" s="60"/>
       <c r="CO3" s="267"/>
+      <c r="CP3" s="267"/>
     </row>
-    <row r="4" spans="1:93" ht="31" thickBot="1">
+    <row r="4" spans="1:94" ht="31" thickBot="1">
       <c r="A4" s="245"/>
       <c r="B4" s="13">
         <v>4</v>
@@ -3684,8 +3714,11 @@
       <c r="CO4" s="268" t="s">
         <v>116</v>
       </c>
+      <c r="CP4" s="268" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="5" spans="1:93" ht="31" thickBot="1">
+    <row r="5" spans="1:94" ht="31" thickBot="1">
       <c r="A5" s="247"/>
       <c r="B5" s="42"/>
       <c r="C5" s="72">
@@ -3867,8 +3900,9 @@
       <c r="CM5" s="59"/>
       <c r="CN5" s="60"/>
       <c r="CO5" s="269"/>
+      <c r="CP5" s="269"/>
     </row>
-    <row r="6" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="6" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A6" s="248"/>
       <c r="B6" s="82">
         <v>5</v>
@@ -3994,8 +4028,11 @@
       <c r="CO6" s="270" t="s">
         <v>117</v>
       </c>
+      <c r="CP6" s="270" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:93" ht="31" thickBot="1">
+    <row r="7" spans="1:94" ht="31" thickBot="1">
       <c r="A7" s="247"/>
       <c r="B7" s="13"/>
       <c r="C7" s="72">
@@ -4173,8 +4210,9 @@
       <c r="CM7" s="47"/>
       <c r="CN7" s="50"/>
       <c r="CO7" s="271"/>
+      <c r="CP7" s="271"/>
     </row>
-    <row r="8" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="8" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A8" s="245"/>
       <c r="B8" s="82">
         <v>6</v>
@@ -4292,8 +4330,11 @@
       <c r="CO8" s="265" t="s">
         <v>118</v>
       </c>
+      <c r="CP8" s="265" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="9" spans="1:93" ht="31" thickBot="1">
+    <row r="9" spans="1:94" ht="31" thickBot="1">
       <c r="A9" s="246"/>
       <c r="B9" s="42"/>
       <c r="C9" s="72">
@@ -4479,8 +4520,9 @@
       <c r="CM9" s="59"/>
       <c r="CN9" s="60"/>
       <c r="CO9" s="269"/>
+      <c r="CP9" s="269"/>
     </row>
-    <row r="10" spans="1:93" ht="37" thickTop="1" thickBot="1">
+    <row r="10" spans="1:94" ht="37" thickTop="1" thickBot="1">
       <c r="A10" s="245"/>
       <c r="B10" s="13">
         <v>7</v>
@@ -4598,8 +4640,11 @@
       <c r="CO10" s="270" t="s">
         <v>119</v>
       </c>
+      <c r="CP10" s="270" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="11" spans="1:93" ht="31" thickBot="1">
+    <row r="11" spans="1:94" ht="31" thickBot="1">
       <c r="A11" s="246"/>
       <c r="B11" s="13"/>
       <c r="C11" s="43">
@@ -4781,8 +4826,9 @@
       <c r="CM11" s="47"/>
       <c r="CN11" s="50"/>
       <c r="CO11" s="271"/>
+      <c r="CP11" s="271"/>
     </row>
-    <row r="12" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="12" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A12" s="247"/>
       <c r="B12" s="82">
         <v>8</v>
@@ -4896,8 +4942,11 @@
       <c r="CO12" s="265" t="s">
         <v>120</v>
       </c>
+      <c r="CP12" s="265" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="13" spans="1:93" ht="31" thickBot="1">
+    <row r="13" spans="1:94" ht="31" thickBot="1">
       <c r="A13" s="246"/>
       <c r="B13" s="13"/>
       <c r="C13" s="102">
@@ -5067,8 +5116,9 @@
       <c r="CM13" s="59"/>
       <c r="CN13" s="60"/>
       <c r="CO13" s="269"/>
+      <c r="CP13" s="269"/>
     </row>
-    <row r="14" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="14" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A14" s="247"/>
       <c r="B14" s="82">
         <v>9</v>
@@ -5180,8 +5230,9 @@
       <c r="CM14" s="70"/>
       <c r="CN14" s="71"/>
       <c r="CO14" s="265"/>
+      <c r="CP14" s="265"/>
     </row>
-    <row r="15" spans="1:93" ht="31" thickBot="1">
+    <row r="15" spans="1:94" ht="31" thickBot="1">
       <c r="A15" s="247"/>
       <c r="B15" s="42"/>
       <c r="C15" s="43">
@@ -5347,8 +5398,9 @@
       <c r="CM15" s="59"/>
       <c r="CN15" s="60"/>
       <c r="CO15" s="269"/>
+      <c r="CP15" s="269"/>
     </row>
-    <row r="16" spans="1:93" ht="37" thickTop="1" thickBot="1">
+    <row r="16" spans="1:94" ht="37" thickTop="1" thickBot="1">
       <c r="A16" s="245"/>
       <c r="B16" s="106">
         <v>10</v>
@@ -5462,8 +5514,9 @@
       <c r="CM16" s="97"/>
       <c r="CN16" s="101"/>
       <c r="CO16" s="265"/>
+      <c r="CP16" s="265"/>
     </row>
-    <row r="17" spans="1:93" ht="31" thickBot="1">
+    <row r="17" spans="1:94" ht="31" thickBot="1">
       <c r="A17" s="246"/>
       <c r="B17" s="13"/>
       <c r="C17" s="72">
@@ -5641,8 +5694,9 @@
       <c r="CM17" s="59"/>
       <c r="CN17" s="60"/>
       <c r="CO17" s="269"/>
+      <c r="CP17" s="269"/>
     </row>
-    <row r="18" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="18" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A18" s="245"/>
       <c r="B18" s="82">
         <v>11</v>
@@ -5754,8 +5808,9 @@
       <c r="CM18" s="97"/>
       <c r="CN18" s="101"/>
       <c r="CO18" s="265"/>
+      <c r="CP18" s="265"/>
     </row>
-    <row r="19" spans="1:93" ht="31" thickBot="1">
+    <row r="19" spans="1:94" ht="31" thickBot="1">
       <c r="A19" s="247"/>
       <c r="B19" s="42"/>
       <c r="C19" s="102">
@@ -5913,8 +5968,9 @@
       <c r="CM19" s="59"/>
       <c r="CN19" s="60"/>
       <c r="CO19" s="269"/>
+      <c r="CP19" s="269"/>
     </row>
-    <row r="20" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="20" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A20" s="245"/>
       <c r="B20" s="13">
         <v>12</v>
@@ -6030,8 +6086,9 @@
       <c r="CM20" s="70"/>
       <c r="CN20" s="71"/>
       <c r="CO20" s="265"/>
+      <c r="CP20" s="265"/>
     </row>
-    <row r="21" spans="1:93" ht="31" thickBot="1">
+    <row r="21" spans="1:94" ht="31" thickBot="1">
       <c r="A21" s="246"/>
       <c r="B21" s="13"/>
       <c r="C21" s="72">
@@ -6221,8 +6278,9 @@
       <c r="CM21" s="59"/>
       <c r="CN21" s="60"/>
       <c r="CO21" s="269"/>
+      <c r="CP21" s="269"/>
     </row>
-    <row r="22" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="22" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A22" s="247"/>
       <c r="B22" s="82">
         <v>13</v>
@@ -6338,8 +6396,9 @@
       <c r="CM22" s="70"/>
       <c r="CN22" s="71"/>
       <c r="CO22" s="270"/>
+      <c r="CP22" s="270"/>
     </row>
-    <row r="23" spans="1:93" ht="31" thickBot="1">
+    <row r="23" spans="1:94" ht="31" thickBot="1">
       <c r="A23" s="247"/>
       <c r="B23" s="42"/>
       <c r="C23" s="43">
@@ -6505,8 +6564,9 @@
       <c r="CM23" s="70"/>
       <c r="CN23" s="71"/>
       <c r="CO23" s="271"/>
+      <c r="CP23" s="271"/>
     </row>
-    <row r="24" spans="1:93" ht="37" thickTop="1" thickBot="1">
+    <row r="24" spans="1:94" ht="37" thickTop="1" thickBot="1">
       <c r="A24" s="245"/>
       <c r="B24" s="13">
         <v>14</v>
@@ -6620,8 +6680,9 @@
       <c r="CM24" s="97"/>
       <c r="CN24" s="101"/>
       <c r="CO24" s="270"/>
+      <c r="CP24" s="270"/>
     </row>
-    <row r="25" spans="1:93" ht="31" thickBot="1">
+    <row r="25" spans="1:94" ht="31" thickBot="1">
       <c r="A25" s="246"/>
       <c r="B25" s="117"/>
       <c r="C25" s="118">
@@ -6791,8 +6852,9 @@
       <c r="CM25" s="59"/>
       <c r="CN25" s="60"/>
       <c r="CO25" s="271"/>
+      <c r="CP25" s="271"/>
     </row>
-    <row r="26" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="26" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A26" s="245"/>
       <c r="B26" s="82">
         <v>15</v>
@@ -6904,8 +6966,9 @@
       <c r="CM26" s="70"/>
       <c r="CN26" s="71"/>
       <c r="CO26" s="265"/>
+      <c r="CP26" s="265"/>
     </row>
-    <row r="27" spans="1:93" ht="31" thickBot="1">
+    <row r="27" spans="1:94" ht="31" thickBot="1">
       <c r="A27" s="246"/>
       <c r="B27" s="42"/>
       <c r="C27" s="72">
@@ -7079,8 +7142,9 @@
       <c r="CM27" s="59"/>
       <c r="CN27" s="60"/>
       <c r="CO27" s="269"/>
+      <c r="CP27" s="269"/>
     </row>
-    <row r="28" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="28" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A28" s="248"/>
       <c r="B28" s="82">
         <v>16</v>
@@ -7198,8 +7262,9 @@
       <c r="CM28" s="70"/>
       <c r="CN28" s="71"/>
       <c r="CO28" s="270"/>
+      <c r="CP28" s="270"/>
     </row>
-    <row r="29" spans="1:93" ht="31" thickBot="1">
+    <row r="29" spans="1:94" ht="31" thickBot="1">
       <c r="A29" s="246"/>
       <c r="B29" s="42"/>
       <c r="C29" s="102">
@@ -7385,8 +7450,9 @@
       <c r="CM29" s="70"/>
       <c r="CN29" s="71"/>
       <c r="CO29" s="271"/>
+      <c r="CP29" s="271"/>
     </row>
-    <row r="30" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="30" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A30" s="249"/>
       <c r="B30" s="13">
         <v>17</v>
@@ -7504,8 +7570,9 @@
       <c r="CM30" s="97"/>
       <c r="CN30" s="101"/>
       <c r="CO30" s="265"/>
+      <c r="CP30" s="265"/>
     </row>
-    <row r="31" spans="1:93" ht="31" thickBot="1">
+    <row r="31" spans="1:94" ht="31" thickBot="1">
       <c r="A31" s="247"/>
       <c r="B31" s="13"/>
       <c r="C31" s="123">
@@ -7687,8 +7754,9 @@
       <c r="CM31" s="59"/>
       <c r="CN31" s="60"/>
       <c r="CO31" s="269"/>
+      <c r="CP31" s="269"/>
     </row>
-    <row r="32" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="32" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A32" s="245"/>
       <c r="B32" s="82">
         <v>18</v>
@@ -7802,8 +7870,9 @@
       <c r="CM32" s="70"/>
       <c r="CN32" s="71"/>
       <c r="CO32" s="265"/>
+      <c r="CP32" s="265"/>
     </row>
-    <row r="33" spans="1:93" ht="31" thickBot="1">
+    <row r="33" spans="1:94" ht="31" thickBot="1">
       <c r="A33" s="247"/>
       <c r="B33" s="13"/>
       <c r="C33" s="102">
@@ -7977,8 +8046,9 @@
       <c r="CM33" s="70"/>
       <c r="CN33" s="71"/>
       <c r="CO33" s="269"/>
+      <c r="CP33" s="269"/>
     </row>
-    <row r="34" spans="1:93" ht="37" thickTop="1" thickBot="1">
+    <row r="34" spans="1:94" ht="37" thickTop="1" thickBot="1">
       <c r="A34" s="248"/>
       <c r="B34" s="82">
         <v>19</v>
@@ -8094,8 +8164,9 @@
       <c r="CM34" s="97"/>
       <c r="CN34" s="101"/>
       <c r="CO34" s="270"/>
+      <c r="CP34" s="270"/>
     </row>
-    <row r="35" spans="1:93" ht="31" thickBot="1">
+    <row r="35" spans="1:94" ht="31" thickBot="1">
       <c r="A35" s="247"/>
       <c r="B35" s="13"/>
       <c r="C35" s="72">
@@ -8277,8 +8348,9 @@
       <c r="CM35" s="59"/>
       <c r="CN35" s="60"/>
       <c r="CO35" s="271"/>
+      <c r="CP35" s="271"/>
     </row>
-    <row r="36" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="36" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A36" s="248"/>
       <c r="B36" s="82">
         <v>20</v>
@@ -8394,8 +8466,9 @@
       <c r="CM36" s="125"/>
       <c r="CN36" s="126"/>
       <c r="CO36" s="270"/>
+      <c r="CP36" s="270"/>
     </row>
-    <row r="37" spans="1:93" ht="31" thickBot="1">
+    <row r="37" spans="1:94" ht="31" thickBot="1">
       <c r="A37" s="247"/>
       <c r="B37" s="13"/>
       <c r="C37" s="72">
@@ -8553,8 +8626,9 @@
       <c r="CM37" s="59"/>
       <c r="CN37" s="60"/>
       <c r="CO37" s="271"/>
+      <c r="CP37" s="271"/>
     </row>
-    <row r="38" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="38" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A38" s="248"/>
       <c r="B38" s="82">
         <v>21</v>
@@ -8670,8 +8744,9 @@
       <c r="CM38" s="70"/>
       <c r="CN38" s="71"/>
       <c r="CO38" s="270"/>
+      <c r="CP38" s="270"/>
     </row>
-    <row r="39" spans="1:93" ht="31" thickBot="1">
+    <row r="39" spans="1:94" ht="31" thickBot="1">
       <c r="A39" s="247"/>
       <c r="B39" s="42"/>
       <c r="C39" s="72">
@@ -8865,8 +8940,9 @@
       <c r="CM39" s="70"/>
       <c r="CN39" s="71"/>
       <c r="CO39" s="271"/>
+      <c r="CP39" s="271"/>
     </row>
-    <row r="40" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="40" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A40" s="245"/>
       <c r="B40" s="82">
         <v>22</v>
@@ -8980,8 +9056,9 @@
       <c r="CM40" s="97"/>
       <c r="CN40" s="101"/>
       <c r="CO40" s="265"/>
+      <c r="CP40" s="265"/>
     </row>
-    <row r="41" spans="1:93" ht="31" thickBot="1">
+    <row r="41" spans="1:94" ht="31" thickBot="1">
       <c r="A41" s="247"/>
       <c r="B41" s="42"/>
       <c r="C41" s="43">
@@ -9171,8 +9248,9 @@
       <c r="CM41" s="59"/>
       <c r="CN41" s="60"/>
       <c r="CO41" s="269"/>
+      <c r="CP41" s="269"/>
     </row>
-    <row r="42" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="42" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A42" s="245"/>
       <c r="B42" s="82">
         <v>23</v>
@@ -9282,8 +9360,9 @@
       <c r="CM42" s="135"/>
       <c r="CN42" s="101"/>
       <c r="CO42" s="265"/>
+      <c r="CP42" s="265"/>
     </row>
-    <row r="43" spans="1:93" ht="31" thickBot="1">
+    <row r="43" spans="1:94" ht="31" thickBot="1">
       <c r="A43" s="250"/>
       <c r="B43" s="13"/>
       <c r="C43" s="43">
@@ -9453,8 +9532,9 @@
       <c r="CM43" s="125"/>
       <c r="CN43" s="71"/>
       <c r="CO43" s="269"/>
+      <c r="CP43" s="269"/>
     </row>
-    <row r="44" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="44" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A44" s="247"/>
       <c r="B44" s="82">
         <v>24</v>
@@ -9566,8 +9646,9 @@
       <c r="CM44" s="97"/>
       <c r="CN44" s="101"/>
       <c r="CO44" s="270"/>
+      <c r="CP44" s="270"/>
     </row>
-    <row r="45" spans="1:93" ht="31" thickBot="1">
+    <row r="45" spans="1:94" ht="31" thickBot="1">
       <c r="A45" s="246"/>
       <c r="B45" s="13"/>
       <c r="C45" s="72">
@@ -9741,8 +9822,9 @@
       <c r="CM45" s="59"/>
       <c r="CN45" s="60"/>
       <c r="CO45" s="271"/>
+      <c r="CP45" s="271"/>
     </row>
-    <row r="46" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="46" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A46" s="245"/>
       <c r="B46" s="82">
         <v>25</v>
@@ -9858,8 +9940,9 @@
       <c r="CM46" s="70"/>
       <c r="CN46" s="71"/>
       <c r="CO46" s="270"/>
+      <c r="CP46" s="270"/>
     </row>
-    <row r="47" spans="1:93" ht="31" thickBot="1">
+    <row r="47" spans="1:94" ht="31" thickBot="1">
       <c r="A47" s="246"/>
       <c r="B47" s="42"/>
       <c r="C47" s="136">
@@ -10029,8 +10112,9 @@
       <c r="CM47" s="59"/>
       <c r="CN47" s="60"/>
       <c r="CO47" s="271"/>
+      <c r="CP47" s="271"/>
     </row>
-    <row r="48" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="48" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A48" s="251"/>
       <c r="B48" s="82">
         <v>26</v>
@@ -10142,8 +10226,9 @@
       <c r="CM48" s="70"/>
       <c r="CN48" s="71"/>
       <c r="CO48" s="265"/>
+      <c r="CP48" s="265"/>
     </row>
-    <row r="49" spans="1:93" ht="31" thickBot="1">
+    <row r="49" spans="1:94" ht="31" thickBot="1">
       <c r="A49" s="247"/>
       <c r="B49" s="42"/>
       <c r="C49" s="72">
@@ -10321,8 +10406,9 @@
       <c r="CM49" s="59"/>
       <c r="CN49" s="60"/>
       <c r="CO49" s="269"/>
+      <c r="CP49" s="269"/>
     </row>
-    <row r="50" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="50" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A50" s="248"/>
       <c r="B50" s="82">
         <v>27</v>
@@ -10434,8 +10520,9 @@
       <c r="CM50" s="70"/>
       <c r="CN50" s="71"/>
       <c r="CO50" s="265"/>
+      <c r="CP50" s="265"/>
     </row>
-    <row r="51" spans="1:93" ht="31" thickBot="1">
+    <row r="51" spans="1:94" ht="31" thickBot="1">
       <c r="A51" s="246"/>
       <c r="B51" s="82"/>
       <c r="C51" s="72">
@@ -10605,8 +10692,9 @@
       <c r="CM51" s="59"/>
       <c r="CN51" s="60"/>
       <c r="CO51" s="269"/>
+      <c r="CP51" s="269"/>
     </row>
-    <row r="52" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="52" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A52" s="247"/>
       <c r="B52" s="82">
         <v>28</v>
@@ -10720,8 +10808,9 @@
       <c r="CM52" s="125"/>
       <c r="CN52" s="71"/>
       <c r="CO52" s="270"/>
+      <c r="CP52" s="270"/>
     </row>
-    <row r="53" spans="1:93" ht="31" thickBot="1">
+    <row r="53" spans="1:94" ht="31" thickBot="1">
       <c r="A53" s="250"/>
       <c r="B53" s="13"/>
       <c r="C53" s="43">
@@ -10891,8 +10980,9 @@
       <c r="CM53" s="140"/>
       <c r="CN53" s="60"/>
       <c r="CO53" s="271"/>
+      <c r="CP53" s="271"/>
     </row>
-    <row r="54" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="54" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A54" s="248"/>
       <c r="B54" s="82">
         <v>29</v>
@@ -11006,8 +11096,9 @@
       <c r="CM54" s="70"/>
       <c r="CN54" s="71"/>
       <c r="CO54" s="270"/>
+      <c r="CP54" s="270"/>
     </row>
-    <row r="55" spans="1:93" ht="31" thickBot="1">
+    <row r="55" spans="1:94" ht="31" thickBot="1">
       <c r="A55" s="246"/>
       <c r="B55" s="13"/>
       <c r="C55" s="72">
@@ -11185,8 +11276,9 @@
       <c r="CM55" s="70"/>
       <c r="CN55" s="71"/>
       <c r="CO55" s="271"/>
+      <c r="CP55" s="271"/>
     </row>
-    <row r="56" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="56" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A56" s="248"/>
       <c r="B56" s="82">
         <v>30</v>
@@ -11302,8 +11394,9 @@
       <c r="CM56" s="97"/>
       <c r="CN56" s="101"/>
       <c r="CO56" s="265"/>
+      <c r="CP56" s="265"/>
     </row>
-    <row r="57" spans="1:93" ht="31" thickBot="1">
+    <row r="57" spans="1:94" ht="31" thickBot="1">
       <c r="A57" s="246"/>
       <c r="B57" s="141"/>
       <c r="C57" s="72">
@@ -11477,8 +11570,9 @@
       <c r="CM57" s="59"/>
       <c r="CN57" s="60"/>
       <c r="CO57" s="269"/>
+      <c r="CP57" s="269"/>
     </row>
-    <row r="58" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="58" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A58" s="248"/>
       <c r="B58" s="82">
         <v>31</v>
@@ -11588,8 +11682,9 @@
       <c r="CM58" s="135"/>
       <c r="CN58" s="101"/>
       <c r="CO58" s="265"/>
+      <c r="CP58" s="265"/>
     </row>
-    <row r="59" spans="1:93" ht="31" thickBot="1">
+    <row r="59" spans="1:94" ht="31" thickBot="1">
       <c r="A59" s="247"/>
       <c r="B59" s="42"/>
       <c r="C59" s="72">
@@ -11747,8 +11842,9 @@
       <c r="CM59" s="140"/>
       <c r="CN59" s="60"/>
       <c r="CO59" s="269"/>
+      <c r="CP59" s="269"/>
     </row>
-    <row r="60" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="60" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A60" s="248"/>
       <c r="B60" s="82">
         <v>32</v>
@@ -11860,8 +11956,9 @@
       <c r="CM60" s="135"/>
       <c r="CN60" s="101"/>
       <c r="CO60" s="265"/>
+      <c r="CP60" s="265"/>
     </row>
-    <row r="61" spans="1:93" ht="31" thickBot="1">
+    <row r="61" spans="1:94" ht="31" thickBot="1">
       <c r="A61" s="246"/>
       <c r="B61" s="42"/>
       <c r="C61" s="43">
@@ -12039,8 +12136,9 @@
       <c r="CM61" s="140"/>
       <c r="CN61" s="60"/>
       <c r="CO61" s="269"/>
+      <c r="CP61" s="269"/>
     </row>
-    <row r="62" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="62" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A62" s="245"/>
       <c r="B62" s="13">
         <v>33</v>
@@ -12154,8 +12252,9 @@
       <c r="CM62" s="125"/>
       <c r="CN62" s="71"/>
       <c r="CO62" s="265"/>
+      <c r="CP62" s="265"/>
     </row>
-    <row r="63" spans="1:93" ht="31" thickBot="1">
+    <row r="63" spans="1:94" ht="31" thickBot="1">
       <c r="A63" s="250"/>
       <c r="B63" s="42"/>
       <c r="C63" s="43">
@@ -12325,8 +12424,9 @@
       <c r="CM63" s="125"/>
       <c r="CN63" s="71"/>
       <c r="CO63" s="269"/>
+      <c r="CP63" s="269"/>
     </row>
-    <row r="64" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="64" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A64" s="252"/>
       <c r="B64" s="13">
         <v>34</v>
@@ -12438,8 +12538,9 @@
       <c r="CM64" s="97"/>
       <c r="CN64" s="101"/>
       <c r="CO64" s="265"/>
+      <c r="CP64" s="265"/>
     </row>
-    <row r="65" spans="1:93" ht="31" thickBot="1">
+    <row r="65" spans="1:94" ht="31" thickBot="1">
       <c r="A65" s="253"/>
       <c r="B65" s="13"/>
       <c r="C65" s="102">
@@ -12601,8 +12702,9 @@
       <c r="CM65" s="59"/>
       <c r="CN65" s="60"/>
       <c r="CO65" s="269"/>
+      <c r="CP65" s="269"/>
     </row>
-    <row r="66" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="66" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A66" s="248"/>
       <c r="B66" s="82">
         <v>35</v>
@@ -12720,8 +12822,9 @@
       <c r="CM66" s="135"/>
       <c r="CN66" s="101"/>
       <c r="CO66" s="265"/>
+      <c r="CP66" s="265"/>
     </row>
-    <row r="67" spans="1:93" ht="31" thickBot="1">
+    <row r="67" spans="1:94" ht="31" thickBot="1">
       <c r="A67" s="246"/>
       <c r="B67" s="143"/>
       <c r="C67" s="144">
@@ -12899,8 +13002,9 @@
       <c r="CM67" s="140"/>
       <c r="CN67" s="60"/>
       <c r="CO67" s="269"/>
+      <c r="CP67" s="269"/>
     </row>
-    <row r="68" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="68" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A68" s="254"/>
       <c r="B68" s="146">
         <v>36</v>
@@ -13014,8 +13118,9 @@
       <c r="CM68" s="135"/>
       <c r="CN68" s="101"/>
       <c r="CO68" s="270"/>
+      <c r="CP68" s="270"/>
     </row>
-    <row r="69" spans="1:93" ht="31" thickBot="1">
+    <row r="69" spans="1:94" ht="31" thickBot="1">
       <c r="A69" s="255"/>
       <c r="B69" s="143"/>
       <c r="C69" s="43">
@@ -13181,8 +13286,9 @@
       <c r="CM69" s="140"/>
       <c r="CN69" s="60"/>
       <c r="CO69" s="271"/>
+      <c r="CP69" s="271"/>
     </row>
-    <row r="70" spans="1:93" ht="31" thickTop="1">
+    <row r="70" spans="1:94" ht="31" thickTop="1">
       <c r="A70" s="256"/>
       <c r="B70" s="149">
         <v>36</v>
@@ -13278,8 +13384,9 @@
       <c r="CM70" s="97"/>
       <c r="CN70" s="101"/>
       <c r="CO70" s="270"/>
+      <c r="CP70" s="270"/>
     </row>
-    <row r="71" spans="1:93" ht="31" thickBot="1">
+    <row r="71" spans="1:94" ht="31" thickBot="1">
       <c r="A71" s="250"/>
       <c r="B71" s="146"/>
       <c r="C71" s="43"/>
@@ -13373,8 +13480,9 @@
       <c r="CM71" s="70"/>
       <c r="CN71" s="71"/>
       <c r="CO71" s="271"/>
+      <c r="CP71" s="271"/>
     </row>
-    <row r="72" spans="1:93" ht="31" thickTop="1">
+    <row r="72" spans="1:94" ht="31" thickTop="1">
       <c r="A72" s="256"/>
       <c r="B72" s="151"/>
       <c r="C72" s="102"/>
@@ -13468,8 +13576,9 @@
       <c r="CM72" s="135"/>
       <c r="CN72" s="101"/>
       <c r="CO72" s="265"/>
+      <c r="CP72" s="265"/>
     </row>
-    <row r="73" spans="1:93" ht="31" thickBot="1">
+    <row r="73" spans="1:94" ht="31" thickBot="1">
       <c r="A73" s="250"/>
       <c r="B73" s="153"/>
       <c r="C73" s="102"/>
@@ -13563,8 +13672,9 @@
       <c r="CM73" s="140"/>
       <c r="CN73" s="60"/>
       <c r="CO73" s="269"/>
+      <c r="CP73" s="269"/>
     </row>
-    <row r="74" spans="1:93" ht="31" thickTop="1">
+    <row r="74" spans="1:94" ht="31" thickTop="1">
       <c r="A74" s="256"/>
       <c r="B74" s="155"/>
       <c r="C74" s="99"/>
@@ -13658,8 +13768,9 @@
       <c r="CM74" s="125"/>
       <c r="CN74" s="71"/>
       <c r="CO74" s="265"/>
+      <c r="CP74" s="265"/>
     </row>
-    <row r="75" spans="1:93" ht="31" thickBot="1">
+    <row r="75" spans="1:94" ht="31" thickBot="1">
       <c r="A75" s="257"/>
       <c r="B75" s="156"/>
       <c r="C75" s="102"/>
@@ -13753,8 +13864,9 @@
       <c r="CM75" s="70"/>
       <c r="CN75" s="71"/>
       <c r="CO75" s="272"/>
+      <c r="CP75" s="272"/>
     </row>
-    <row r="76" spans="1:93" ht="31" thickBot="1">
+    <row r="76" spans="1:94" ht="31" thickBot="1">
       <c r="A76" s="244"/>
       <c r="B76" s="162"/>
       <c r="C76" s="2" t="s">
@@ -13892,26 +14004,27 @@
       <c r="CM76" s="10"/>
       <c r="CN76" s="10"/>
       <c r="CO76" s="273"/>
+      <c r="CP76" s="273"/>
     </row>
-    <row r="77" spans="1:93">
+    <row r="77" spans="1:94">
       <c r="A77" s="258"/>
       <c r="B77" s="165">
         <f>SUM(D2:D75)</f>
-        <v>309</v>
+        <v>299.5</v>
       </c>
       <c r="C77" s="166" t="s">
         <v>104</v>
       </c>
       <c r="D77" s="167">
         <f>SUM(B77)</f>
-        <v>309</v>
+        <v>299.5</v>
       </c>
       <c r="E77" s="168">
         <v>3</v>
       </c>
       <c r="F77" s="169">
         <f>SUM(D77,E78)</f>
-        <v>309</v>
+        <v>299.5</v>
       </c>
       <c r="G77" s="170"/>
       <c r="H77" s="171"/>
@@ -14000,14 +14113,15 @@
       <c r="CM77" s="70"/>
       <c r="CN77" s="40"/>
       <c r="CO77" s="273"/>
+      <c r="CP77" s="273"/>
     </row>
-    <row r="78" spans="1:93" ht="31" thickBot="1">
+    <row r="78" spans="1:94" ht="31" thickBot="1">
       <c r="A78" s="259" t="s">
         <v>105</v>
       </c>
       <c r="B78" s="177">
         <f>SUM(E2:E75)</f>
-        <v>71</v>
+        <v>61.5</v>
       </c>
       <c r="C78" s="178"/>
       <c r="D78" s="179"/>
@@ -14100,8 +14214,9 @@
       <c r="CM78" s="70"/>
       <c r="CN78" s="263"/>
       <c r="CO78" s="273"/>
+      <c r="CP78" s="273"/>
     </row>
-    <row r="79" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="79" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A79" s="260">
         <f>SUM(A80:B80)</f>
         <v>34</v>
@@ -14117,7 +14232,7 @@
       <c r="E79" s="187"/>
       <c r="F79" s="188">
         <f>SUM(F77-B79)</f>
-        <v>71</v>
+        <v>61.5</v>
       </c>
       <c r="G79" s="189"/>
       <c r="H79" s="190"/>
@@ -14142,7 +14257,7 @@
       <c r="W79" s="125"/>
       <c r="X79" s="193">
         <f>F77</f>
-        <v>309</v>
+        <v>299.5</v>
       </c>
       <c r="Y79" s="194"/>
       <c r="Z79" s="195"/>
@@ -14213,8 +14328,9 @@
       <c r="CM79" s="70"/>
       <c r="CN79" s="263"/>
       <c r="CO79" s="273"/>
+      <c r="CP79" s="273"/>
     </row>
-    <row r="80" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="80" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A80" s="261"/>
       <c r="B80" s="199">
         <f>SUM(C2:C75)</f>
@@ -14319,8 +14435,9 @@
       <c r="CM80" s="70"/>
       <c r="CN80" s="263"/>
       <c r="CO80" s="273"/>
+      <c r="CP80" s="273"/>
     </row>
-    <row r="81" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="81" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A81" s="261"/>
       <c r="B81" s="177">
         <f>SUM(D2)</f>
@@ -14353,7 +14470,7 @@
       <c r="W81" s="125"/>
       <c r="X81" s="193">
         <f>F79</f>
-        <v>71</v>
+        <v>61.5</v>
       </c>
       <c r="Y81" s="194"/>
       <c r="Z81" s="195"/>
@@ -14424,8 +14541,9 @@
       <c r="CM81" s="70"/>
       <c r="CN81" s="263"/>
       <c r="CO81" s="273"/>
+      <c r="CP81" s="273"/>
     </row>
-    <row r="82" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="82" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A82" s="260" t="s">
         <v>109</v>
       </c>
@@ -14529,8 +14647,9 @@
       <c r="CM82" s="70"/>
       <c r="CN82" s="263"/>
       <c r="CO82" s="273"/>
+      <c r="CP82" s="273"/>
     </row>
-    <row r="83" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="83" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A83" s="260">
         <f>SUM(A84:B84)</f>
         <v>0</v>
@@ -14637,8 +14756,9 @@
       <c r="CM83" s="70"/>
       <c r="CN83" s="263"/>
       <c r="CO83" s="273"/>
+      <c r="CP83" s="273"/>
     </row>
-    <row r="84" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="84" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A84" s="261"/>
       <c r="B84" s="199">
         <f>SUM(C2)</f>
@@ -14737,8 +14857,9 @@
       <c r="CM84" s="174"/>
       <c r="CN84" s="264"/>
       <c r="CO84" s="273"/>
+      <c r="CP84" s="273"/>
     </row>
-    <row r="85" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="85" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A85" s="261"/>
       <c r="B85" s="222"/>
       <c r="C85" s="223"/>
@@ -14768,7 +14889,7 @@
       <c r="W85" s="125"/>
       <c r="X85" s="228">
         <f>F77/29</f>
-        <v>10.655172413793103</v>
+        <v>10.327586206896552</v>
       </c>
       <c r="Y85" s="229"/>
       <c r="Z85" s="230"/>
@@ -14839,8 +14960,9 @@
       <c r="CM85" s="125"/>
       <c r="CN85" s="263"/>
       <c r="CO85" s="273"/>
+      <c r="CP85" s="273"/>
     </row>
-    <row r="86" spans="1:93" ht="32" thickTop="1" thickBot="1">
+    <row r="86" spans="1:94" ht="32" thickTop="1" thickBot="1">
       <c r="A86" s="262" t="s">
         <v>115</v>
       </c>
@@ -14848,7 +14970,7 @@
       <c r="C86" s="233"/>
       <c r="D86" s="234">
         <f>SUM(D77,D80)</f>
-        <v>309</v>
+        <v>299.5</v>
       </c>
       <c r="E86" s="234">
         <f>SUM(E78,E81)</f>
@@ -14942,6 +15064,7 @@
       <c r="CM86" s="238"/>
       <c r="CN86" s="238"/>
       <c r="CO86" s="273"/>
+      <c r="CP86" s="273"/>
     </row>
   </sheetData>
   <mergeCells count="58">

</xml_diff>